<commit_message>
Modified transitions names, renamed expected status header in _Tests.xlsx, renamed out_Comment.
</commit_message>
<xml_diff>
--- a/Reframework_update/Tests/_Tests.xlsx
+++ b/Reframework_update/Tests/_Tests.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB487D9-46E7-4F34-9F48-9CC8B50E768B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6166F478-4F8B-40F8-8F04-65565652B963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8148" yWindow="-15720" windowWidth="18732" windowHeight="13464" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>WorkflowFile</t>
   </si>
   <si>
-    <t>Exception</t>
-  </si>
-  <si>
     <t>AppEx</t>
   </si>
   <si>
@@ -51,17 +48,20 @@
   </si>
   <si>
     <t>Framework\InitAllApplications.xaml</t>
+  </si>
+  <si>
+    <t>ExpectedResult</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -69,7 +69,7 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -77,13 +77,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -395,85 +395,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="2" width="41.875" customWidth="1"/>
+    <col min="1" max="2" width="41.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
       <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -492,30 +492,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="46.375" customWidth="1"/>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
-    <col min="3" max="3" width="11.375" customWidth="1"/>
-    <col min="4" max="4" width="135.625" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="135.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed exception naming for RunAllTests.
</commit_message>
<xml_diff>
--- a/Reframework_update/Tests/_Tests.xlsx
+++ b/Reframework_update/Tests/_Tests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6166F478-4F8B-40F8-8F04-65565652B963}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C91F313D-6341-4D80-817D-BA6E5DBC36B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8148" yWindow="-15720" windowWidth="18732" windowHeight="13464" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
     <t>WorkflowFile</t>
   </si>
   <si>
-    <t>AppEx</t>
-  </si>
-  <si>
     <t>Success</t>
   </si>
   <si>
@@ -51,6 +48,9 @@
   </si>
   <si>
     <t>ExpectedResult</t>
+  </si>
+  <si>
+    <t>SystemException</t>
   </si>
 </sst>
 </file>
@@ -395,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -409,78 +409,78 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B16" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"Success,BRE,AppEx"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{7198B273-8CEB-4936-858C-3C618DA468FB}">
+      <formula1>"Success,BusinessException,SystemException"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -492,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -509,21 +509,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="3"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>"Success,BRE,AppEx"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{CB13DA15-0017-4E26-927A-C3254031AF44}">
+      <formula1>"Success,BusinessException,SystemException"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>